<commit_message>
Criacao de dados mockados, ajustes no Schedule
</commit_message>
<xml_diff>
--- a/Time_03/Dicionario/Tabelas.xlsx
+++ b/Time_03/Dicionario/Tabelas.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Reserva" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Reserva!$A$1:$G$8</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>RES_Id</t>
   </si>
@@ -32,17 +35,67 @@
   </si>
   <si>
     <t>PLA_Id</t>
+  </si>
+  <si>
+    <t>46070d4bf934fb0d4b06d9e2c46e346944e322444900a435d7d9a95e6d7435f5</t>
+  </si>
+  <si>
+    <t>5abecfd3a447514b314339a6</t>
+  </si>
+  <si>
+    <t>5adfdcaf860f6f45cee4c6c4</t>
+  </si>
+  <si>
+    <t>5aef92b8124bc3b4db6932b7</t>
+  </si>
+  <si>
+    <t>ESP_ID</t>
+  </si>
+  <si>
+    <t>12340d4bf934fb0d4b06d9e2c46e346944e322444900a435d7d9a95e6d7435a1</t>
+  </si>
+  <si>
+    <t>12340d4bf934fb0d4b06d9e2c46e346944e322444900a435d7d9a95e6d7435a2</t>
+  </si>
+  <si>
+    <t>12340d4bf934fb0d4b06d9e2c46e346944e322444900a435d7d9a95e6d7435a3</t>
+  </si>
+  <si>
+    <t>12340d4bf934fb0d4b06d9e2c46e346944e322444900a435d7d9a95e6d7435a4</t>
+  </si>
+  <si>
+    <t>12340d4bf934fb0d4b06d9e2c46e346944e322444900a435d7d9a95e6d7435a5</t>
+  </si>
+  <si>
+    <t>5abecfd3a447514b314339a7</t>
+  </si>
+  <si>
+    <t>5abecfd3a447514b314339a8</t>
+  </si>
+  <si>
+    <t>5abecfd3a447514b314339a9</t>
+  </si>
+  <si>
+    <t>5abecfd3a447514b314339a10</t>
+  </si>
+  <si>
+    <t>12340d4bf934fb0d4b06d9e2c46e346944e322444900a435d7d9a95e6d7435a6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ hh:mm"/>
-  </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -70,9 +123,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,25 +427,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="24" style="1" customWidth="1"/>
+    <col min="2" max="3" width="24" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -397,68 +460,185 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="57.6">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>43229.568379629629</v>
-      </c>
-      <c r="C2" s="1">
-        <v>43229.656574074077</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="B2" s="2">
+        <v>43266.75</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43266.833333333336</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="57.6">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>43229.693379629629</v>
-      </c>
-      <c r="C3" s="1">
-        <v>43229.735046296293</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="B3" s="2">
+        <v>43266.708333333336</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43266.75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="57.6">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>43229.375011574077</v>
-      </c>
-      <c r="C4" s="1">
-        <v>43229.500011574077</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
+      <c r="B4" s="2">
+        <v>43266.833333333336</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43266.875</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="57.6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>43266.770833333336</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43266.8125</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="57.6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>43266.875</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43266.916666666664</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="57.6">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>43266.916666666664</v>
+      </c>
+      <c r="C7" s="3">
+        <v>43266.958333333336</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="1">
+        <v>123456</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="129.6">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>43266.958333333336</v>
+      </c>
+      <c r="C8" s="3">
+        <v>43267.083333333336</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="1">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G8">
+    <filterColumn colId="5"/>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Inclusao de novas informaçoes Mockadas
</commit_message>
<xml_diff>
--- a/Time_03/Dicionario/Tabelas.xlsx
+++ b/Time_03/Dicionario/Tabelas.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Reserva" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Reserva!$A$1:$G$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Reserva!$A$1:$H$8</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>RES_Id</t>
   </si>
@@ -80,13 +80,115 @@
   </si>
   <si>
     <t>12340d4bf934fb0d4b06d9e2c46e346944e322444900a435d7d9a95e6d7435a6</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>AB+</t>
+  </si>
+  <si>
+    <t>O-</t>
+  </si>
+  <si>
+    <t>O+</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>heartbeat</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Patient 1</t>
+  </si>
+  <si>
+    <t>Patient 2</t>
+  </si>
+  <si>
+    <t>Patient 3</t>
+  </si>
+  <si>
+    <t>Patient 4</t>
+  </si>
+  <si>
+    <t>Patient 5</t>
+  </si>
+  <si>
+    <t>Patient 6</t>
+  </si>
+  <si>
+    <t>Patient 7</t>
+  </si>
+  <si>
+    <t>wound</t>
+  </si>
+  <si>
+    <t>manchester</t>
+  </si>
+  <si>
+    <t>body_part</t>
+  </si>
+  <si>
+    <t>Fratura</t>
+  </si>
+  <si>
+    <t>Cabeça</t>
+  </si>
+  <si>
+    <t>Membros Inferiores</t>
+  </si>
+  <si>
+    <t>Membros Superiores</t>
+  </si>
+  <si>
+    <t>Coluna</t>
+  </si>
+  <si>
+    <t>Pelve</t>
+  </si>
+  <si>
+    <t>Abdômen</t>
+  </si>
+  <si>
+    <t>Pescoço</t>
+  </si>
+  <si>
+    <t>Escoriação</t>
+  </si>
+  <si>
+    <t>Contusão</t>
+  </si>
+  <si>
+    <t>Traumatismo</t>
+  </si>
+  <si>
+    <t>Hematoma</t>
+  </si>
+  <si>
+    <t>Luxação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -95,12 +197,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -123,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -132,7 +240,16 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,217 +544,413 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <sheetPr codeName="Plan1"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomRight" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="24" style="2" customWidth="1"/>
+    <col min="3" max="4" width="24" style="2" customWidth="1"/>
+    <col min="5" max="7" width="13.44140625" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="57.6">
-      <c r="A2">
+    <row r="2" spans="1:15">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5">
         <v>43266.75</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="5">
         <v>43266.833333333336</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="4">
         <v>123456</v>
       </c>
+      <c r="I2" s="4">
+        <v>30</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="4">
+        <v>36.6</v>
+      </c>
+      <c r="L2" s="4">
+        <v>80</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="9">
+        <v>2</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="57.6">
-      <c r="A3">
+    <row r="3" spans="1:15">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="5">
         <v>43266.708333333336</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="5">
         <v>43266.75</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="4">
         <v>123456</v>
       </c>
+      <c r="I3" s="4">
+        <v>40</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="4">
+        <v>36.5</v>
+      </c>
+      <c r="L3" s="4">
+        <v>75</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="9">
+        <v>3</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="57.6">
-      <c r="A4">
+    <row r="4" spans="1:15">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5">
         <v>43266.833333333336</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="5">
         <v>43266.875</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="4">
         <v>123456</v>
       </c>
+      <c r="I4" s="4">
+        <v>50</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="4">
+        <v>38.5</v>
+      </c>
+      <c r="L4" s="4">
+        <v>75</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="9">
+        <v>1</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="57.6">
-      <c r="A5">
+    <row r="5" spans="1:15">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="5">
         <v>43266.770833333336</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="5">
         <v>43266.8125</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="4">
         <v>123456</v>
       </c>
+      <c r="I5" s="4">
+        <v>38</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="4">
+        <v>36.6</v>
+      </c>
+      <c r="L5" s="4">
+        <v>90</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="9">
+        <v>4</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" ht="57.6">
-      <c r="A6">
+    <row r="6" spans="1:15">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="5">
         <v>43266.875</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="5">
         <v>43266.916666666664</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="4">
         <v>123456</v>
       </c>
+      <c r="I6" s="4">
+        <v>42</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="4">
+        <v>36.5</v>
+      </c>
+      <c r="L6" s="4">
+        <v>88</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" s="9">
+        <v>3</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" ht="57.6">
-      <c r="A7" s="1">
+    <row r="7" spans="1:15">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="5">
         <v>43266.916666666664</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="5">
         <v>43266.958333333336</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="4">
         <v>123456</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="I7" s="7">
+        <v>25</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="4">
+        <v>40</v>
+      </c>
+      <c r="L7" s="4">
+        <v>80</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" s="9">
+        <v>2</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" ht="129.6">
-      <c r="A8" s="1">
+    <row r="8" spans="1:15">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="5">
         <v>43266.958333333336</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="5">
         <v>43267.083333333336</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="4">
         <v>123456</v>
       </c>
+      <c r="I8" s="4">
+        <v>66</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="4">
+        <v>36.6</v>
+      </c>
+      <c r="L8" s="4">
+        <v>120</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="9">
+        <v>5</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:15">
       <c r="A9" s="1"/>
-      <c r="B9" s="3"/>
+      <c r="B9" s="1"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G8">
-    <filterColumn colId="5"/>
+  <autoFilter ref="A1:H8">
+    <filterColumn colId="1"/>
+    <filterColumn colId="6"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Comunicacao Cross e Painel
</commit_message>
<xml_diff>
--- a/Time_03/Dicionario/Tabelas.xlsx
+++ b/Time_03/Dicionario/Tabelas.xlsx
@@ -115,27 +115,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Patient 1</t>
-  </si>
-  <si>
-    <t>Patient 2</t>
-  </si>
-  <si>
-    <t>Patient 3</t>
-  </si>
-  <si>
-    <t>Patient 4</t>
-  </si>
-  <si>
-    <t>Patient 5</t>
-  </si>
-  <si>
-    <t>Patient 6</t>
-  </si>
-  <si>
-    <t>Patient 7</t>
-  </si>
-  <si>
     <t>wound</t>
   </si>
   <si>
@@ -182,6 +161,27 @@
   </si>
   <si>
     <t>Luxação</t>
+  </si>
+  <si>
+    <t>Paciente 1</t>
+  </si>
+  <si>
+    <t>Paciente 2</t>
+  </si>
+  <si>
+    <t>Paciente 3</t>
+  </si>
+  <si>
+    <t>Paciente 4</t>
+  </si>
+  <si>
+    <t>Paciente 5</t>
+  </si>
+  <si>
+    <t>Paciente 6</t>
+  </si>
+  <si>
+    <t>Paciente 7</t>
   </si>
 </sst>
 </file>
@@ -551,13 +551,16 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N19" sqref="N19"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="24" style="2" customWidth="1"/>
-    <col min="5" max="7" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -599,13 +602,13 @@
         <v>30</v>
       </c>
       <c r="M1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="N1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="O1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -613,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5">
         <v>43266.75</v>
@@ -646,13 +649,13 @@
         <v>80</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="N2" s="9">
         <v>2</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -660,7 +663,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C3" s="5">
         <v>43266.708333333336</v>
@@ -693,13 +696,13 @@
         <v>75</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N3" s="9">
         <v>3</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -707,7 +710,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C4" s="5">
         <v>43266.833333333336</v>
@@ -722,7 +725,7 @@
         <v>17</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H4" s="4">
         <v>123456</v>
@@ -740,13 +743,13 @@
         <v>75</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="N4" s="9">
         <v>1</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -754,7 +757,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C5" s="5">
         <v>43266.770833333336</v>
@@ -787,13 +790,13 @@
         <v>90</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="N5" s="9">
         <v>4</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -801,7 +804,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C6" s="5">
         <v>43266.875</v>
@@ -816,7 +819,7 @@
         <v>19</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H6" s="4">
         <v>123456</v>
@@ -834,13 +837,13 @@
         <v>88</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="N6" s="9">
         <v>3</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -848,13 +851,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C7" s="5">
-        <v>43266.916666666664</v>
+        <v>43266.958333333336</v>
       </c>
       <c r="D7" s="5">
-        <v>43266.958333333336</v>
+        <v>43267.041666666664</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>20</v>
@@ -881,13 +884,13 @@
         <v>80</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="N7" s="9">
         <v>2</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -895,7 +898,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C8" s="5">
         <v>43266.958333333336</v>
@@ -928,13 +931,13 @@
         <v>120</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="N8" s="9">
         <v>5</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:15">

</xml_diff>